<commit_message>
test resorces changed according to logic changes
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/AutoFilter/CustomAutoFilter.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/AutoFilter/CustomAutoFilter.xlsx
@@ -95,12 +95,12 @@
     </x:border>
   </x:borders>
   <x:cellStyleXfs count="1">
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
   </x:cellStyleXfs>
   <x:cellXfs count="1">
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>

</xml_diff>